<commit_message>
update BUKU TA  bab 5
</commit_message>
<xml_diff>
--- a/Buku TA/Uji Coba.xlsx
+++ b/Buku TA/Uji Coba.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Static Buffer" sheetId="1" r:id="rId1"/>
     <sheet name="Dinamic Buffer" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="69">
   <si>
     <t>0 x</t>
   </si>
@@ -197,13 +198,43 @@
   </si>
   <si>
     <t>AVG</t>
+  </si>
+  <si>
+    <t>Panjang Data</t>
+  </si>
+  <si>
+    <t>homogen</t>
+  </si>
+  <si>
+    <t>heterogen</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Waktu Kompresi Data</t>
+  </si>
+  <si>
+    <t>Waktu Dekompresi Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">efektifitas </t>
+  </si>
+  <si>
+    <t>efektifitas</t>
+  </si>
+  <si>
+    <t>tA</t>
+  </si>
+  <si>
+    <t>tB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +258,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,7 +345,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -446,12 +485,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -508,32 +573,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -571,26 +630,80 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -909,32 +1022,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="K2" s="36" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="K2" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
     </row>
     <row r="3" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
         <v>1</v>
@@ -951,10 +1064,10 @@
       <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="38"/>
+      <c r="L3" s="56"/>
       <c r="M3" s="14"/>
       <c r="N3" s="15" t="s">
         <v>1</v>
@@ -973,10 +1086,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="39">
+      <c r="A4" s="37">
         <v>584</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -995,10 +1108,10 @@
       <c r="H4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="39">
+      <c r="K4" s="37">
         <v>584</v>
       </c>
-      <c r="L4" s="40"/>
+      <c r="L4" s="38"/>
       <c r="M4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1019,8 +1132,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1039,8 +1152,8 @@
       <c r="H5" s="1">
         <v>21</v>
       </c>
-      <c r="K5" s="41"/>
-      <c r="L5" s="42"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="40"/>
       <c r="M5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1061,8 +1174,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1086,8 +1199,8 @@
         <f>($A$4-H5)/$A$4</f>
         <v>0.96404109589041098</v>
       </c>
-      <c r="K6" s="41"/>
-      <c r="L6" s="42"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
       <c r="M6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1113,8 +1226,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1133,8 +1246,8 @@
       <c r="H7" s="1">
         <v>427</v>
       </c>
-      <c r="K7" s="41"/>
-      <c r="L7" s="42"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="40"/>
       <c r="M7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1155,8 +1268,8 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1180,8 +1293,8 @@
         <f>($A$4-H7)/$A$4</f>
         <v>0.26883561643835618</v>
       </c>
-      <c r="K8" s="43"/>
-      <c r="L8" s="44"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1207,10 +1320,10 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="45">
+      <c r="A9" s="43">
         <v>980</v>
       </c>
-      <c r="B9" s="46"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="16" t="s">
         <v>30</v>
       </c>
@@ -1229,10 +1342,10 @@
       <c r="H9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="45">
+      <c r="K9" s="43">
         <v>980</v>
       </c>
-      <c r="L9" s="46"/>
+      <c r="L9" s="44"/>
       <c r="M9" s="16" t="s">
         <v>30</v>
       </c>
@@ -1253,8 +1366,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="48"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="16" t="s">
         <v>21</v>
       </c>
@@ -1273,8 +1386,8 @@
       <c r="H10" s="16">
         <v>33</v>
       </c>
-      <c r="K10" s="47"/>
-      <c r="L10" s="48"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="16" t="s">
         <v>21</v>
       </c>
@@ -1295,8 +1408,8 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="48"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
@@ -1320,8 +1433,8 @@
         <f>($A$9-H10)/$A$9</f>
         <v>0.96632653061224494</v>
       </c>
-      <c r="K11" s="47"/>
-      <c r="L11" s="48"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="46"/>
       <c r="M11" s="16" t="s">
         <v>35</v>
       </c>
@@ -1347,8 +1460,8 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="48"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="16" t="s">
         <v>22</v>
       </c>
@@ -1367,8 +1480,8 @@
       <c r="H12" s="16">
         <v>564</v>
       </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="48"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
       <c r="M12" s="16" t="s">
         <v>22</v>
       </c>
@@ -1389,8 +1502,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="16" t="s">
         <v>34</v>
       </c>
@@ -1414,8 +1527,8 @@
         <f>($A$9-H12)/$A$9</f>
         <v>0.42448979591836733</v>
       </c>
-      <c r="K13" s="49"/>
-      <c r="L13" s="50"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
       <c r="M13" s="16" t="s">
         <v>34</v>
       </c>
@@ -1441,10 +1554,10 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="49">
         <v>1280</v>
       </c>
-      <c r="B14" s="31"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>30</v>
       </c>
@@ -1463,10 +1576,10 @@
       <c r="H14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="30">
+      <c r="K14" s="49">
         <v>1280</v>
       </c>
-      <c r="L14" s="31"/>
+      <c r="L14" s="50"/>
       <c r="M14" s="13" t="s">
         <v>30</v>
       </c>
@@ -1487,8 +1600,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
@@ -1505,8 +1618,8 @@
         <v>68</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="52"/>
       <c r="M15" s="4" t="s">
         <v>21</v>
       </c>
@@ -1527,8 +1640,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1552,8 +1665,8 @@
         <f>($A$14-H15)/$A$14</f>
         <v>1</v>
       </c>
-      <c r="K16" s="32"/>
-      <c r="L16" s="33"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="52"/>
       <c r="M16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1579,8 +1692,8 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="51"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1597,8 +1710,8 @@
         <v>1120</v>
       </c>
       <c r="H17" s="5"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="33"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="52"/>
       <c r="M17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1619,8 +1732,8 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1644,8 +1757,8 @@
         <f>($A$14-H17)/$A$14</f>
         <v>1</v>
       </c>
-      <c r="K18" s="34"/>
-      <c r="L18" s="35"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="54"/>
       <c r="M18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1671,10 +1784,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="51">
+      <c r="A19" s="30">
         <v>1345</v>
       </c>
-      <c r="B19" s="52"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="7" t="s">
         <v>30</v>
       </c>
@@ -1693,10 +1806,10 @@
       <c r="H19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K19" s="51">
+      <c r="K19" s="30">
         <v>1345</v>
       </c>
-      <c r="L19" s="52"/>
+      <c r="L19" s="31"/>
       <c r="M19" s="7" t="s">
         <v>30</v>
       </c>
@@ -1717,8 +1830,8 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
@@ -1735,8 +1848,8 @@
         <v>129</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="54"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="33"/>
       <c r="M20" s="7" t="s">
         <v>21</v>
       </c>
@@ -1757,8 +1870,8 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="7" t="s">
         <v>35</v>
       </c>
@@ -1779,8 +1892,8 @@
         <v>0.90408921933085507</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="54"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="33"/>
       <c r="M21" s="7" t="s">
         <v>35</v>
       </c>
@@ -1806,8 +1919,8 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="54"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
@@ -1824,8 +1937,8 @@
         <v>1182</v>
       </c>
       <c r="H22" s="5"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="54"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="33"/>
       <c r="M22" s="7" t="s">
         <v>22</v>
       </c>
@@ -1844,8 +1957,8 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="56"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="7" t="s">
         <v>34</v>
       </c>
@@ -1866,8 +1979,8 @@
         <v>0.12118959107806691</v>
       </c>
       <c r="H23" s="5"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="56"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="35"/>
       <c r="M23" s="7" t="s">
         <v>34</v>
       </c>
@@ -1890,10 +2003,10 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K24" s="57">
+      <c r="K24" s="36">
         <v>1640</v>
       </c>
-      <c r="L24" s="57"/>
+      <c r="L24" s="36"/>
       <c r="M24" s="24" t="s">
         <v>30</v>
       </c>
@@ -1914,10 +2027,10 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
         <v>1</v>
@@ -1934,10 +2047,10 @@
       <c r="H28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="37" t="s">
+      <c r="K28" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="L28" s="38"/>
+      <c r="L28" s="56"/>
       <c r="M28" s="14"/>
       <c r="N28" s="15" t="s">
         <v>1</v>
@@ -1956,10 +2069,10 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="39">
+      <c r="A29" s="37">
         <v>584</v>
       </c>
-      <c r="B29" s="40"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1979,10 +2092,10 @@
         <v>8.1119999999999994E-3</v>
       </c>
       <c r="J29" s="24"/>
-      <c r="K29" s="39">
+      <c r="K29" s="37">
         <v>584</v>
       </c>
-      <c r="L29" s="40"/>
+      <c r="L29" s="38"/>
       <c r="M29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2003,8 +2116,8 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="1" t="s">
         <v>24</v>
       </c>
@@ -2023,8 +2136,8 @@
       <c r="H30" s="1">
         <v>3.248E-3</v>
       </c>
-      <c r="K30" s="41"/>
-      <c r="L30" s="42"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="40"/>
       <c r="M30" s="1" t="s">
         <v>24</v>
       </c>
@@ -2045,8 +2158,8 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="42"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="19" t="s">
         <v>32</v>
       </c>
@@ -2070,8 +2183,8 @@
         <f t="shared" si="0"/>
         <v>1.1359999999999999E-2</v>
       </c>
-      <c r="K31" s="41"/>
-      <c r="L31" s="42"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="40"/>
       <c r="M31" s="19" t="s">
         <v>32</v>
       </c>
@@ -2097,8 +2210,8 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
@@ -2118,8 +2231,8 @@
         <v>4.0691999999999999E-2</v>
       </c>
       <c r="J32" s="24"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="42"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="40"/>
       <c r="M32" s="1" t="s">
         <v>25</v>
       </c>
@@ -2140,8 +2253,8 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="1" t="s">
         <v>26</v>
       </c>
@@ -2160,8 +2273,8 @@
       <c r="H33" s="1">
         <v>1.7328E-2</v>
       </c>
-      <c r="K33" s="41"/>
-      <c r="L33" s="42"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="40"/>
       <c r="M33" s="1" t="s">
         <v>26</v>
       </c>
@@ -2182,8 +2295,8 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="44"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="19" t="s">
         <v>32</v>
       </c>
@@ -2207,8 +2320,8 @@
         <f t="shared" si="2"/>
         <v>5.8020000000000002E-2</v>
       </c>
-      <c r="K34" s="43"/>
-      <c r="L34" s="44"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="42"/>
       <c r="M34" s="19" t="s">
         <v>32</v>
       </c>
@@ -2234,10 +2347,10 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="45">
+      <c r="A35" s="43">
         <v>980</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="44"/>
       <c r="C35" s="16" t="s">
         <v>23</v>
       </c>
@@ -2257,10 +2370,10 @@
         <v>1.2716E-2</v>
       </c>
       <c r="J35" s="24"/>
-      <c r="K35" s="45">
+      <c r="K35" s="43">
         <v>980</v>
       </c>
-      <c r="L35" s="46"/>
+      <c r="L35" s="44"/>
       <c r="M35" s="16" t="s">
         <v>23</v>
       </c>
@@ -2281,8 +2394,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="48"/>
+      <c r="A36" s="45"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="16" t="s">
         <v>24</v>
       </c>
@@ -2301,8 +2414,8 @@
       <c r="H36" s="16">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="K36" s="47"/>
-      <c r="L36" s="48"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="46"/>
       <c r="M36" s="16" t="s">
         <v>24</v>
       </c>
@@ -2323,8 +2436,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
-      <c r="B37" s="48"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="46"/>
       <c r="C37" s="19" t="s">
         <v>32</v>
       </c>
@@ -2348,8 +2461,8 @@
         <f t="shared" si="4"/>
         <v>1.7916000000000001E-2</v>
       </c>
-      <c r="K37" s="47"/>
-      <c r="L37" s="48"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="46"/>
       <c r="M37" s="19" t="s">
         <v>32</v>
       </c>
@@ -2375,8 +2488,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
-      <c r="B38" s="48"/>
+      <c r="A38" s="45"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="16" t="s">
         <v>25</v>
       </c>
@@ -2396,8 +2509,8 @@
         <v>5.5975999999999998E-2</v>
       </c>
       <c r="J38" s="24"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="48"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="46"/>
       <c r="M38" s="16" t="s">
         <v>25</v>
       </c>
@@ -2418,8 +2531,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
-      <c r="B39" s="48"/>
+      <c r="A39" s="45"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="16" t="s">
         <v>26</v>
       </c>
@@ -2438,8 +2551,8 @@
       <c r="H39" s="16">
         <v>2.3768000000000001E-2</v>
       </c>
-      <c r="K39" s="47"/>
-      <c r="L39" s="48"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="46"/>
       <c r="M39" s="16" t="s">
         <v>26</v>
       </c>
@@ -2460,8 +2573,8 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="19" t="s">
         <v>32</v>
       </c>
@@ -2485,8 +2598,8 @@
         <f t="shared" si="6"/>
         <v>7.9743999999999995E-2</v>
       </c>
-      <c r="K40" s="49"/>
-      <c r="L40" s="50"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="48"/>
       <c r="M40" s="19" t="s">
         <v>32</v>
       </c>
@@ -2512,10 +2625,10 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="30">
+      <c r="A41" s="49">
         <v>1280</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="4" t="s">
         <v>23</v>
       </c>
@@ -2533,10 +2646,10 @@
       </c>
       <c r="H41" s="5"/>
       <c r="J41" s="24"/>
-      <c r="K41" s="30">
+      <c r="K41" s="49">
         <v>1280</v>
       </c>
-      <c r="L41" s="31"/>
+      <c r="L41" s="50"/>
       <c r="M41" s="4" t="s">
         <v>23</v>
       </c>
@@ -2557,8 +2670,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="51"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="4" t="s">
         <v>24</v>
       </c>
@@ -2575,8 +2688,8 @@
         <v>9.476E-3</v>
       </c>
       <c r="H42" s="5"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="33"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="52"/>
       <c r="M42" s="4" t="s">
         <v>24</v>
       </c>
@@ -2597,8 +2710,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="19" t="s">
         <v>32</v>
       </c>
@@ -2619,8 +2732,8 @@
         <v>2.7875999999999998E-2</v>
       </c>
       <c r="H43" s="5"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="33"/>
+      <c r="K43" s="51"/>
+      <c r="L43" s="52"/>
       <c r="M43" s="19" t="s">
         <v>32</v>
       </c>
@@ -2646,8 +2759,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="4" t="s">
         <v>25</v>
       </c>
@@ -2665,8 +2778,8 @@
       </c>
       <c r="H44" s="5"/>
       <c r="J44" s="24"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="33"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="52"/>
       <c r="M44" s="4" t="s">
         <v>25</v>
       </c>
@@ -2687,8 +2800,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="51"/>
+      <c r="B45" s="52"/>
       <c r="C45" s="4" t="s">
         <v>26</v>
       </c>
@@ -2705,8 +2818,8 @@
         <v>4.3580000000000001E-2</v>
       </c>
       <c r="H45" s="5"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="33"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="52"/>
       <c r="M45" s="4" t="s">
         <v>26</v>
       </c>
@@ -2727,8 +2840,8 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="19" t="s">
         <v>32</v>
       </c>
@@ -2749,8 +2862,8 @@
         <v>0.146428</v>
       </c>
       <c r="H46" s="5"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="35"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="54"/>
       <c r="M46" s="19" t="s">
         <v>32</v>
       </c>
@@ -2776,10 +2889,10 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="51">
+      <c r="A47" s="30">
         <v>1345</v>
       </c>
-      <c r="B47" s="52"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="7" t="s">
         <v>23</v>
       </c>
@@ -2797,10 +2910,10 @@
       </c>
       <c r="H47" s="5"/>
       <c r="J47" s="24"/>
-      <c r="K47" s="51">
+      <c r="K47" s="30">
         <v>1345</v>
       </c>
-      <c r="L47" s="52"/>
+      <c r="L47" s="31"/>
       <c r="M47" s="7" t="s">
         <v>23</v>
       </c>
@@ -2821,8 +2934,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="53"/>
-      <c r="B48" s="54"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="33"/>
       <c r="C48" s="7" t="s">
         <v>24</v>
       </c>
@@ -2839,8 +2952,8 @@
         <v>9.9319999999999999E-3</v>
       </c>
       <c r="H48" s="5"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="54"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="33"/>
       <c r="M48" s="7" t="s">
         <v>24</v>
       </c>
@@ -2859,8 +2972,8 @@
       <c r="R48" s="5"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="53"/>
-      <c r="B49" s="54"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="33"/>
       <c r="C49" s="19" t="s">
         <v>32</v>
       </c>
@@ -2881,8 +2994,8 @@
         <v>2.8931999999999999E-2</v>
       </c>
       <c r="H49" s="5"/>
-      <c r="K49" s="53"/>
-      <c r="L49" s="54"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="33"/>
       <c r="M49" s="19" t="s">
         <v>32</v>
       </c>
@@ -2905,8 +3018,8 @@
       <c r="R49" s="5"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="53"/>
-      <c r="B50" s="54"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="7" t="s">
         <v>25</v>
       </c>
@@ -2924,8 +3037,8 @@
       </c>
       <c r="H50" s="5"/>
       <c r="J50" s="24"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="54"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="33"/>
       <c r="M50" s="7" t="s">
         <v>25</v>
       </c>
@@ -2944,8 +3057,8 @@
       <c r="R50" s="5"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="53"/>
-      <c r="B51" s="54"/>
+      <c r="A51" s="32"/>
+      <c r="B51" s="33"/>
       <c r="C51" s="7" t="s">
         <v>26</v>
       </c>
@@ -2962,8 +3075,8 @@
         <v>4.5887999999999998E-2</v>
       </c>
       <c r="H51" s="5"/>
-      <c r="K51" s="53"/>
-      <c r="L51" s="54"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="33"/>
       <c r="M51" s="7" t="s">
         <v>26</v>
       </c>
@@ -2982,8 +3095,8 @@
       <c r="R51" s="5"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="55"/>
-      <c r="B52" s="56"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="35"/>
       <c r="C52" s="19" t="s">
         <v>32</v>
       </c>
@@ -3004,8 +3117,8 @@
         <v>0.15465999999999999</v>
       </c>
       <c r="H52" s="5"/>
-      <c r="K52" s="55"/>
-      <c r="L52" s="56"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="35"/>
       <c r="M52" s="19" t="s">
         <v>32</v>
       </c>
@@ -3029,6 +3142,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K41:L46"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L8"/>
+    <mergeCell ref="K9:L13"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="K47:L52"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="A47:B52"/>
@@ -3045,13 +3165,6 @@
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="K29:L34"/>
     <mergeCell ref="K35:L40"/>
-    <mergeCell ref="K41:L46"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L8"/>
-    <mergeCell ref="K9:L13"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3062,8 +3175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:B40"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,32 +3202,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15" t="s">
         <v>1</v>
@@ -3163,10 +3276,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="39">
+      <c r="A3" s="37">
         <v>584</v>
       </c>
-      <c r="B3" s="40"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
@@ -3217,8 +3330,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
@@ -3269,8 +3382,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -3336,8 +3449,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
@@ -3388,8 +3501,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
@@ -3455,10 +3568,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="45">
+      <c r="A8" s="43">
         <v>980</v>
       </c>
-      <c r="B8" s="46"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="16" t="s">
         <v>30</v>
       </c>
@@ -3509,8 +3622,8 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
@@ -3561,8 +3674,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="48"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="16" t="s">
         <v>35</v>
       </c>
@@ -3628,8 +3741,8 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="48"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="16" t="s">
         <v>22</v>
       </c>
@@ -3680,8 +3793,8 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="16" t="s">
         <v>34</v>
       </c>
@@ -3747,10 +3860,10 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="49">
         <v>1280</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
@@ -3801,8 +3914,8 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
@@ -3853,8 +3966,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
@@ -3920,8 +4033,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
@@ -3972,8 +4085,8 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
@@ -4039,10 +4152,10 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="51">
+      <c r="A18" s="30">
         <v>1345</v>
       </c>
-      <c r="B18" s="52"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="7" t="s">
         <v>30</v>
       </c>
@@ -4096,8 +4209,8 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="54"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="7" t="s">
         <v>21</v>
       </c>
@@ -4151,8 +4264,8 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="7" t="s">
         <v>35</v>
       </c>
@@ -4218,8 +4331,8 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="7" t="s">
         <v>22</v>
       </c>
@@ -4270,8 +4383,8 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="56"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
@@ -4337,10 +4450,10 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="57">
+      <c r="A23" s="36">
         <v>1640</v>
       </c>
-      <c r="B23" s="57"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="24" t="s">
         <v>30</v>
       </c>
@@ -4371,10 +4484,10 @@
       <c r="R23" s="25"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
         <v>1</v>
@@ -4432,10 +4545,10 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="39">
+      <c r="A29" s="37">
         <v>584</v>
       </c>
-      <c r="B29" s="40"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
@@ -4486,8 +4599,8 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="1" t="s">
         <v>24</v>
       </c>
@@ -4538,8 +4651,8 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="42"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="19" t="s">
         <v>32</v>
       </c>
@@ -4605,8 +4718,8 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
@@ -4657,8 +4770,8 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="1" t="s">
         <v>26</v>
       </c>
@@ -4709,8 +4822,8 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="44"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="19" t="s">
         <v>32</v>
       </c>
@@ -4776,10 +4889,10 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="45">
+      <c r="A35" s="43">
         <v>980</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="44"/>
       <c r="C35" s="16" t="s">
         <v>23</v>
       </c>
@@ -4830,8 +4943,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="48"/>
+      <c r="A36" s="45"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="16" t="s">
         <v>24</v>
       </c>
@@ -4882,8 +4995,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
-      <c r="B37" s="48"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="46"/>
       <c r="C37" s="19" t="s">
         <v>32</v>
       </c>
@@ -4949,8 +5062,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
-      <c r="B38" s="48"/>
+      <c r="A38" s="45"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="16" t="s">
         <v>25</v>
       </c>
@@ -5001,8 +5114,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
-      <c r="B39" s="48"/>
+      <c r="A39" s="45"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="16" t="s">
         <v>26</v>
       </c>
@@ -5053,8 +5166,8 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="19" t="s">
         <v>32</v>
       </c>
@@ -5120,10 +5233,10 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="30">
+      <c r="A41" s="49">
         <v>1280</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="4" t="s">
         <v>23</v>
       </c>
@@ -5174,8 +5287,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="51"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="4" t="s">
         <v>24</v>
       </c>
@@ -5226,8 +5339,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="19" t="s">
         <v>32</v>
       </c>
@@ -5293,8 +5406,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="4" t="s">
         <v>25</v>
       </c>
@@ -5345,8 +5458,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="51"/>
+      <c r="B45" s="52"/>
       <c r="C45" s="4" t="s">
         <v>26</v>
       </c>
@@ -5397,8 +5510,8 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="19" t="s">
         <v>32</v>
       </c>
@@ -5464,10 +5577,10 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="51">
+      <c r="A47" s="30">
         <v>1345</v>
       </c>
-      <c r="B47" s="52"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="7" t="s">
         <v>23</v>
       </c>
@@ -5518,8 +5631,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="53"/>
-      <c r="B48" s="54"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="33"/>
       <c r="C48" s="7" t="s">
         <v>24</v>
       </c>
@@ -5570,8 +5683,8 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="53"/>
-      <c r="B49" s="54"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="33"/>
       <c r="C49" s="19" t="s">
         <v>32</v>
       </c>
@@ -5637,8 +5750,8 @@
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="53"/>
-      <c r="B50" s="54"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="7" t="s">
         <v>25</v>
       </c>
@@ -5689,8 +5802,8 @@
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="53"/>
-      <c r="B51" s="54"/>
+      <c r="A51" s="32"/>
+      <c r="B51" s="33"/>
       <c r="C51" s="7" t="s">
         <v>26</v>
       </c>
@@ -5741,8 +5854,8 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="55"/>
-      <c r="B52" s="56"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="35"/>
       <c r="C52" s="19" t="s">
         <v>32</v>
       </c>
@@ -5824,4 +5937,846 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B6:R38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="4" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="6.85546875" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="71">
+        <v>584</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.1028000000000002E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.3664000000000001E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.0004000000000001E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8.7279999999999996E-3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8.0800000000000004E-3</v>
+      </c>
+      <c r="L8" s="58">
+        <v>584</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="1">
+        <v>76</v>
+      </c>
+      <c r="O8" s="1">
+        <v>49</v>
+      </c>
+      <c r="P8" s="1">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>20</v>
+      </c>
+      <c r="R8" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="71"/>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6.1112E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5.3887999999999998E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5.2519999999999997E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5.1184E-2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4.5935999999999998E-2</v>
+      </c>
+      <c r="L9" s="59"/>
+      <c r="M9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="2">
+        <f>($L$8-N8)/$L$8</f>
+        <v>0.86986301369863017</v>
+      </c>
+      <c r="O9" s="2">
+        <f>($L$8-O8)/$L$8</f>
+        <v>0.91609589041095896</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" ref="P9:R9" si="0">($L$8-P8)/$L$8</f>
+        <v>0.94691780821917804</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.96575342465753422</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.97773972602739723</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="72">
+        <v>980</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="16">
+        <v>3.5128E-2</v>
+      </c>
+      <c r="E10" s="16">
+        <v>2.2716E-2</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1.6028000000000001E-2</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1.3391999999999999E-2</v>
+      </c>
+      <c r="H10" s="16">
+        <v>1.2456E-2</v>
+      </c>
+      <c r="L10" s="59"/>
+      <c r="M10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="1">
+        <v>569</v>
+      </c>
+      <c r="O10" s="1">
+        <v>537</v>
+      </c>
+      <c r="P10" s="1">
+        <v>523</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>529</v>
+      </c>
+      <c r="R10" s="1">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="72"/>
+      <c r="C11" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.102136</v>
+      </c>
+      <c r="E11" s="16">
+        <v>9.1095999999999996E-2</v>
+      </c>
+      <c r="F11" s="16">
+        <v>8.6596000000000006E-2</v>
+      </c>
+      <c r="G11" s="16">
+        <v>8.8356000000000004E-2</v>
+      </c>
+      <c r="H11" s="16">
+        <v>6.3119999999999996E-2</v>
+      </c>
+      <c r="L11" s="60"/>
+      <c r="M11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N11" s="2">
+        <f>($L$8-N10)/$L$8</f>
+        <v>2.5684931506849314E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" ref="O11:R11" si="1">($L$8-O10)/$L$8</f>
+        <v>8.0479452054794523E-2</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.10445205479452055</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="1"/>
+        <v>9.4178082191780824E-2</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.2363013698630137</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="73">
+        <v>1280</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4.5724000000000001E-2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.9187999999999999E-2</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2.0747999999999999E-2</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1.6704E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="L12" s="61">
+        <v>980</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="16">
+        <v>126</v>
+      </c>
+      <c r="O12" s="16">
+        <v>80</v>
+      </c>
+      <c r="P12" s="16">
+        <v>49</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>31</v>
+      </c>
+      <c r="R12" s="16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="73"/>
+      <c r="C13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.13236000000000001</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.11812400000000001</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.113096</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.111024</v>
+      </c>
+      <c r="H13" s="4">
+        <v>6.6844000000000001E-2</v>
+      </c>
+      <c r="L13" s="62"/>
+      <c r="M13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="18">
+        <f>($L$12-N12)/$L$12</f>
+        <v>0.87142857142857144</v>
+      </c>
+      <c r="O13" s="18">
+        <f t="shared" ref="O13:R13" si="2">($L$12-O12)/$L$12</f>
+        <v>0.91836734693877553</v>
+      </c>
+      <c r="P13" s="18">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="Q13" s="18">
+        <f t="shared" si="2"/>
+        <v>0.96836734693877546</v>
+      </c>
+      <c r="R13" s="18">
+        <f t="shared" si="2"/>
+        <v>0.98061224489795917</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="69">
+        <v>1345</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3.0632E-2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2.1752000000000001E-2</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1.7176E-2</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1.5807999999999999E-2</v>
+      </c>
+      <c r="L14" s="62"/>
+      <c r="M14" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N14" s="16">
+        <v>947</v>
+      </c>
+      <c r="O14" s="16">
+        <v>917</v>
+      </c>
+      <c r="P14" s="16">
+        <v>905</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>912</v>
+      </c>
+      <c r="R14" s="16">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="69"/>
+      <c r="C15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.138604</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.124512</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.11898</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.11692</v>
+      </c>
+      <c r="H15" s="7">
+        <v>6.7227999999999996E-2</v>
+      </c>
+      <c r="L15" s="63"/>
+      <c r="M15" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="N15" s="18">
+        <f>($L$12-N14)/$L$12</f>
+        <v>3.3673469387755103E-2</v>
+      </c>
+      <c r="O15" s="18">
+        <f t="shared" ref="O15:R15" si="3">($L$12-O14)/$L$12</f>
+        <v>6.4285714285714279E-2</v>
+      </c>
+      <c r="P15" s="18">
+        <f t="shared" si="3"/>
+        <v>7.6530612244897961E-2</v>
+      </c>
+      <c r="Q15" s="18">
+        <f t="shared" si="3"/>
+        <v>6.9387755102040816E-2</v>
+      </c>
+      <c r="R15" s="18">
+        <f t="shared" si="3"/>
+        <v>0.40714285714285714</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L16" s="64">
+        <v>1280</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" s="4">
+        <v>163</v>
+      </c>
+      <c r="O16" s="22">
+        <v>103</v>
+      </c>
+      <c r="P16" s="22">
+        <v>63</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>38</v>
+      </c>
+      <c r="R16" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L17" s="65"/>
+      <c r="M17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N17" s="6">
+        <f>($L$16-N16)/$L$16</f>
+        <v>0.87265625000000002</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" ref="O17:R17" si="4">($L$16-O16)/$L$16</f>
+        <v>0.91953125000000002</v>
+      </c>
+      <c r="P17" s="6">
+        <f t="shared" si="4"/>
+        <v>0.95078125000000002</v>
+      </c>
+      <c r="Q17" s="6">
+        <f t="shared" si="4"/>
+        <v>0.97031250000000002</v>
+      </c>
+      <c r="R17" s="6">
+        <f t="shared" si="4"/>
+        <v>0.98203125000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L18" s="65"/>
+      <c r="M18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1223</v>
+      </c>
+      <c r="O18" s="22">
+        <v>1193</v>
+      </c>
+      <c r="P18" s="22">
+        <v>1181</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>1138</v>
+      </c>
+      <c r="R18" s="4">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L19" s="66"/>
+      <c r="M19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N19" s="6">
+        <f>($L$16-N18)/$L$16</f>
+        <v>4.4531250000000001E-2</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" ref="O19:R19" si="5">($L$16-O18)/$L$16</f>
+        <v>6.7968749999999994E-2</v>
+      </c>
+      <c r="P19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.7343750000000003E-2</v>
+      </c>
+      <c r="Q19" s="6">
+        <f>($L$16-Q18)/$L$16</f>
+        <v>0.11093749999999999</v>
+      </c>
+      <c r="R19" s="6">
+        <f t="shared" si="5"/>
+        <v>0.53671875000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L20" s="69">
+        <v>1345</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="7">
+        <v>171</v>
+      </c>
+      <c r="O20" s="7">
+        <v>108</v>
+      </c>
+      <c r="P20" s="7">
+        <v>66</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>39</v>
+      </c>
+      <c r="R20" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L21" s="69"/>
+      <c r="M21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="N21" s="8">
+        <f>($L$20-N20)/$L$20</f>
+        <v>0.87286245353159853</v>
+      </c>
+      <c r="O21" s="8">
+        <f t="shared" ref="O21:R21" si="6">($L$20-O20)/$L$20</f>
+        <v>0.91970260223048328</v>
+      </c>
+      <c r="P21" s="8">
+        <f t="shared" si="6"/>
+        <v>0.95092936802973982</v>
+      </c>
+      <c r="Q21" s="8">
+        <f t="shared" si="6"/>
+        <v>0.971003717472119</v>
+      </c>
+      <c r="R21" s="8">
+        <f t="shared" si="6"/>
+        <v>0.98141263940520451</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L22" s="69"/>
+      <c r="M22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N22" s="7">
+        <v>1282</v>
+      </c>
+      <c r="O22" s="7">
+        <v>1254</v>
+      </c>
+      <c r="P22" s="7">
+        <v>1243</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>1201</v>
+      </c>
+      <c r="R22" s="7">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L23" s="69"/>
+      <c r="M23" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="N23" s="8">
+        <f>($L$20-N22)/$L$20</f>
+        <v>4.6840148698884761E-2</v>
+      </c>
+      <c r="O23" s="8">
+        <f t="shared" ref="O23:R23" si="7">($L$20-O22)/$L$20</f>
+        <v>6.7657992565055766E-2</v>
+      </c>
+      <c r="P23" s="8">
+        <f t="shared" si="7"/>
+        <v>7.5836431226765796E-2</v>
+      </c>
+      <c r="Q23" s="8">
+        <f t="shared" si="7"/>
+        <v>0.10706319702602231</v>
+      </c>
+      <c r="R23" s="8">
+        <f t="shared" si="7"/>
+        <v>0.55985130111524162</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="71">
+        <v>584</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="1">
+        <v>7.2519999999999998E-3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4.5640000000000003E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3.6480000000000002E-3</v>
+      </c>
+      <c r="G31" s="1">
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2.944E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="71"/>
+      <c r="C32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2.1187999999999999E-2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2.0572E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2.0671999999999999E-2</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1.7288000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="72">
+        <v>980</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="16">
+        <v>1.2004000000000001E-2</v>
+      </c>
+      <c r="E33" s="16">
+        <v>8.9280000000000002E-3</v>
+      </c>
+      <c r="F33" s="16">
+        <v>5.9040000000000004E-3</v>
+      </c>
+      <c r="G33" s="16">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="H33" s="16">
+        <v>4.6759999999999996E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="72"/>
+      <c r="C34" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="16">
+        <v>3.5228000000000002E-2</v>
+      </c>
+      <c r="E34" s="16">
+        <v>3.4680000000000002E-2</v>
+      </c>
+      <c r="F34" s="16">
+        <v>3.4556000000000003E-2</v>
+      </c>
+      <c r="G34" s="16">
+        <v>3.4079999999999999E-2</v>
+      </c>
+      <c r="H34" s="16">
+        <v>2.3528E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="73">
+        <v>1280</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1.558E-2</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1.1552E-2</v>
+      </c>
+      <c r="F35" s="4">
+        <v>9.3480000000000004E-3</v>
+      </c>
+      <c r="G35" s="4">
+        <v>6.5120000000000004E-3</v>
+      </c>
+      <c r="H35" s="4">
+        <v>5.9719999999999999E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="73"/>
+      <c r="C36" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="4">
+        <v>4.5443999999999998E-2</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4.4943999999999998E-2</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.4847999999999999E-2</v>
+      </c>
+      <c r="G36" s="4">
+        <v>4.3816000000000001E-2</v>
+      </c>
+      <c r="H36" s="4">
+        <v>2.5492000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="69">
+        <v>1345</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1.6407999999999999E-2</v>
+      </c>
+      <c r="E37" s="7">
+        <v>1.2156E-2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>9.8840000000000004E-3</v>
+      </c>
+      <c r="G37" s="7">
+        <v>6.8079999999999998E-3</v>
+      </c>
+      <c r="H37" s="7">
+        <v>6.2960000000000004E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="69"/>
+      <c r="C38" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="7">
+        <v>4.7668000000000002E-2</v>
+      </c>
+      <c r="E38" s="7">
+        <v>4.7224000000000002E-2</v>
+      </c>
+      <c r="F38" s="7">
+        <v>4.7156000000000003E-2</v>
+      </c>
+      <c r="G38" s="7">
+        <v>4.6131999999999999E-2</v>
+      </c>
+      <c r="H38" s="7">
+        <v>2.5832000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update hasil uji coba
</commit_message>
<xml_diff>
--- a/Buku TA/Uji Coba.xlsx
+++ b/Buku TA/Uji Coba.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E503EDB-5B65-4D8E-AE4F-0D7D8A3F0023}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Static Buffer" sheetId="1" r:id="rId1"/>
     <sheet name="Dinamic Buffer" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Akurasi Pengiriman" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="95">
   <si>
     <t>0 x</t>
   </si>
@@ -306,11 +306,35 @@
   <si>
     <t>error</t>
   </si>
+  <si>
+    <t>Jarak</t>
+  </si>
+  <si>
+    <t>5 meter</t>
+  </si>
+  <si>
+    <t>10 meter</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>20 meter</t>
+  </si>
+  <si>
+    <t>30 meter</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -605,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -690,26 +714,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -747,31 +777,25 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,18 +814,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -831,12 +843,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,7 +1150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R52"/>
   <sheetViews>
     <sheetView topLeftCell="I26" workbookViewId="0">
@@ -1154,32 +1182,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="K2" s="69" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="K2" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
     </row>
     <row r="3" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="68"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
         <v>1</v>
@@ -1196,10 +1224,10 @@
       <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="67" t="s">
+      <c r="K3" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="68"/>
+      <c r="L3" s="50"/>
       <c r="M3" s="14"/>
       <c r="N3" s="15" t="s">
         <v>1</v>
@@ -1218,10 +1246,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="49">
+      <c r="A4" s="51">
         <v>584</v>
       </c>
-      <c r="B4" s="50"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1240,10 +1268,10 @@
       <c r="H4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="49">
+      <c r="K4" s="51">
         <v>584</v>
       </c>
-      <c r="L4" s="50"/>
+      <c r="L4" s="52"/>
       <c r="M4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1264,8 +1292,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1284,8 +1312,8 @@
       <c r="H5" s="1">
         <v>21</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="52"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="54"/>
       <c r="M5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1306,8 +1334,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1331,8 +1359,8 @@
         <f>($A$4-H5)/$A$4</f>
         <v>0.96404109589041098</v>
       </c>
-      <c r="K6" s="51"/>
-      <c r="L6" s="52"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="54"/>
       <c r="M6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1358,8 +1386,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1378,8 +1406,8 @@
       <c r="H7" s="1">
         <v>427</v>
       </c>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="54"/>
       <c r="M7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1400,8 +1428,8 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="54"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1425,8 +1453,8 @@
         <f>($A$4-H7)/$A$4</f>
         <v>0.26883561643835618</v>
       </c>
-      <c r="K8" s="53"/>
-      <c r="L8" s="54"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
       <c r="M8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1452,10 +1480,10 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="55">
+      <c r="A9" s="57">
         <v>980</v>
       </c>
-      <c r="B9" s="56"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="16" t="s">
         <v>30</v>
       </c>
@@ -1474,10 +1502,10 @@
       <c r="H9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="55">
+      <c r="K9" s="57">
         <v>980</v>
       </c>
-      <c r="L9" s="56"/>
+      <c r="L9" s="58"/>
       <c r="M9" s="16" t="s">
         <v>30</v>
       </c>
@@ -1498,8 +1526,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="58"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="16" t="s">
         <v>21</v>
       </c>
@@ -1518,8 +1546,8 @@
       <c r="H10" s="16">
         <v>33</v>
       </c>
-      <c r="K10" s="57"/>
-      <c r="L10" s="58"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="60"/>
       <c r="M10" s="16" t="s">
         <v>21</v>
       </c>
@@ -1540,8 +1568,8 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
@@ -1565,8 +1593,8 @@
         <f>($A$9-H10)/$A$9</f>
         <v>0.96632653061224494</v>
       </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="58"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="16" t="s">
         <v>35</v>
       </c>
@@ -1592,8 +1620,8 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
-      <c r="B12" s="58"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="16" t="s">
         <v>22</v>
       </c>
@@ -1612,8 +1640,8 @@
       <c r="H12" s="16">
         <v>564</v>
       </c>
-      <c r="K12" s="57"/>
-      <c r="L12" s="58"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="60"/>
       <c r="M12" s="16" t="s">
         <v>22</v>
       </c>
@@ -1634,8 +1662,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="60"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="16" t="s">
         <v>34</v>
       </c>
@@ -1659,8 +1687,8 @@
         <f>($A$9-H12)/$A$9</f>
         <v>0.42448979591836733</v>
       </c>
-      <c r="K13" s="59"/>
-      <c r="L13" s="60"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="62"/>
       <c r="M13" s="16" t="s">
         <v>34</v>
       </c>
@@ -1686,10 +1714,10 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="61">
+      <c r="A14" s="42">
         <v>1280</v>
       </c>
-      <c r="B14" s="62"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="13" t="s">
         <v>30</v>
       </c>
@@ -1708,10 +1736,10 @@
       <c r="H14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="61">
+      <c r="K14" s="42">
         <v>1280</v>
       </c>
-      <c r="L14" s="62"/>
+      <c r="L14" s="43"/>
       <c r="M14" s="13" t="s">
         <v>30</v>
       </c>
@@ -1732,8 +1760,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="64"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
@@ -1750,8 +1778,8 @@
         <v>68</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="64"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
       <c r="M15" s="4" t="s">
         <v>21</v>
       </c>
@@ -1772,8 +1800,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="63"/>
-      <c r="B16" s="64"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1797,8 +1825,8 @@
         <f>($A$14-H15)/$A$14</f>
         <v>1</v>
       </c>
-      <c r="K16" s="63"/>
-      <c r="L16" s="64"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="45"/>
       <c r="M16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1824,8 +1852,8 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1842,8 +1870,8 @@
         <v>1120</v>
       </c>
       <c r="H17" s="5"/>
-      <c r="K17" s="63"/>
-      <c r="L17" s="64"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="45"/>
       <c r="M17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1864,8 +1892,8 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
-      <c r="B18" s="66"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1889,8 +1917,8 @@
         <f>($A$14-H17)/$A$14</f>
         <v>1</v>
       </c>
-      <c r="K18" s="65"/>
-      <c r="L18" s="66"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="47"/>
       <c r="M18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1916,10 +1944,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="42">
+      <c r="A19" s="63">
         <v>1345</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="7" t="s">
         <v>30</v>
       </c>
@@ -1938,10 +1966,10 @@
       <c r="H19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="63">
         <v>1345</v>
       </c>
-      <c r="L19" s="43"/>
+      <c r="L19" s="64"/>
       <c r="M19" s="7" t="s">
         <v>30</v>
       </c>
@@ -1962,8 +1990,8 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
@@ -1980,8 +2008,8 @@
         <v>129</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="45"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="66"/>
       <c r="M20" s="7" t="s">
         <v>21</v>
       </c>
@@ -2002,8 +2030,8 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="7" t="s">
         <v>35</v>
       </c>
@@ -2024,8 +2052,8 @@
         <v>0.90408921933085507</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="45"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="66"/>
       <c r="M21" s="7" t="s">
         <v>35</v>
       </c>
@@ -2051,8 +2079,8 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="45"/>
+      <c r="A22" s="65"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
@@ -2069,8 +2097,8 @@
         <v>1182</v>
       </c>
       <c r="H22" s="5"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="45"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="66"/>
       <c r="M22" s="7" t="s">
         <v>22</v>
       </c>
@@ -2089,8 +2117,8 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="7" t="s">
         <v>34</v>
       </c>
@@ -2111,8 +2139,8 @@
         <v>0.12118959107806691</v>
       </c>
       <c r="H23" s="5"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="47"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="68"/>
       <c r="M23" s="7" t="s">
         <v>34</v>
       </c>
@@ -2135,10 +2163,10 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K24" s="48">
+      <c r="K24" s="69">
         <v>1640</v>
       </c>
-      <c r="L24" s="48"/>
+      <c r="L24" s="69"/>
       <c r="M24" s="24" t="s">
         <v>30</v>
       </c>
@@ -2159,10 +2187,10 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="68"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
         <v>1</v>
@@ -2179,10 +2207,10 @@
       <c r="H28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="67" t="s">
+      <c r="K28" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="L28" s="68"/>
+      <c r="L28" s="50"/>
       <c r="M28" s="14"/>
       <c r="N28" s="15" t="s">
         <v>1</v>
@@ -2201,10 +2229,10 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="49">
+      <c r="A29" s="51">
         <v>584</v>
       </c>
-      <c r="B29" s="50"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2224,10 +2252,10 @@
         <v>8.1119999999999994E-3</v>
       </c>
       <c r="J29" s="24"/>
-      <c r="K29" s="49">
+      <c r="K29" s="51">
         <v>584</v>
       </c>
-      <c r="L29" s="50"/>
+      <c r="L29" s="52"/>
       <c r="M29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2248,8 +2276,8 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="51"/>
-      <c r="B30" s="52"/>
+      <c r="A30" s="53"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="1" t="s">
         <v>24</v>
       </c>
@@ -2268,8 +2296,8 @@
       <c r="H30" s="1">
         <v>3.248E-3</v>
       </c>
-      <c r="K30" s="51"/>
-      <c r="L30" s="52"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="54"/>
       <c r="M30" s="1" t="s">
         <v>24</v>
       </c>
@@ -2290,8 +2318,8 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
+      <c r="A31" s="53"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="19" t="s">
         <v>32</v>
       </c>
@@ -2315,8 +2343,8 @@
         <f t="shared" si="0"/>
         <v>1.1359999999999999E-2</v>
       </c>
-      <c r="K31" s="51"/>
-      <c r="L31" s="52"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="54"/>
       <c r="M31" s="19" t="s">
         <v>32</v>
       </c>
@@ -2342,8 +2370,8 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
@@ -2363,8 +2391,8 @@
         <v>4.0691999999999999E-2</v>
       </c>
       <c r="J32" s="24"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="52"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="54"/>
       <c r="M32" s="1" t="s">
         <v>25</v>
       </c>
@@ -2385,8 +2413,8 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="51"/>
-      <c r="B33" s="52"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="1" t="s">
         <v>26</v>
       </c>
@@ -2405,8 +2433,8 @@
       <c r="H33" s="1">
         <v>1.7328E-2</v>
       </c>
-      <c r="K33" s="51"/>
-      <c r="L33" s="52"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="54"/>
       <c r="M33" s="1" t="s">
         <v>26</v>
       </c>
@@ -2427,8 +2455,8 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="54"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="19" t="s">
         <v>32</v>
       </c>
@@ -2452,8 +2480,8 @@
         <f t="shared" si="2"/>
         <v>5.8020000000000002E-2</v>
       </c>
-      <c r="K34" s="53"/>
-      <c r="L34" s="54"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="56"/>
       <c r="M34" s="19" t="s">
         <v>32</v>
       </c>
@@ -2479,10 +2507,10 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="55">
+      <c r="A35" s="57">
         <v>980</v>
       </c>
-      <c r="B35" s="56"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="16" t="s">
         <v>23</v>
       </c>
@@ -2502,10 +2530,10 @@
         <v>1.2716E-2</v>
       </c>
       <c r="J35" s="24"/>
-      <c r="K35" s="55">
+      <c r="K35" s="57">
         <v>980</v>
       </c>
-      <c r="L35" s="56"/>
+      <c r="L35" s="58"/>
       <c r="M35" s="16" t="s">
         <v>23</v>
       </c>
@@ -2526,8 +2554,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="57"/>
-      <c r="B36" s="58"/>
+      <c r="A36" s="59"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="16" t="s">
         <v>24</v>
       </c>
@@ -2546,8 +2574,8 @@
       <c r="H36" s="16">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="K36" s="57"/>
-      <c r="L36" s="58"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="60"/>
       <c r="M36" s="16" t="s">
         <v>24</v>
       </c>
@@ -2568,8 +2596,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="57"/>
-      <c r="B37" s="58"/>
+      <c r="A37" s="59"/>
+      <c r="B37" s="60"/>
       <c r="C37" s="19" t="s">
         <v>32</v>
       </c>
@@ -2593,8 +2621,8 @@
         <f t="shared" si="4"/>
         <v>1.7916000000000001E-2</v>
       </c>
-      <c r="K37" s="57"/>
-      <c r="L37" s="58"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="60"/>
       <c r="M37" s="19" t="s">
         <v>32</v>
       </c>
@@ -2620,8 +2648,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="57"/>
-      <c r="B38" s="58"/>
+      <c r="A38" s="59"/>
+      <c r="B38" s="60"/>
       <c r="C38" s="16" t="s">
         <v>25</v>
       </c>
@@ -2641,8 +2669,8 @@
         <v>5.5975999999999998E-2</v>
       </c>
       <c r="J38" s="24"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="58"/>
+      <c r="K38" s="59"/>
+      <c r="L38" s="60"/>
       <c r="M38" s="16" t="s">
         <v>25</v>
       </c>
@@ -2663,8 +2691,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="57"/>
-      <c r="B39" s="58"/>
+      <c r="A39" s="59"/>
+      <c r="B39" s="60"/>
       <c r="C39" s="16" t="s">
         <v>26</v>
       </c>
@@ -2683,8 +2711,8 @@
       <c r="H39" s="16">
         <v>2.3768000000000001E-2</v>
       </c>
-      <c r="K39" s="57"/>
-      <c r="L39" s="58"/>
+      <c r="K39" s="59"/>
+      <c r="L39" s="60"/>
       <c r="M39" s="16" t="s">
         <v>26</v>
       </c>
@@ -2705,8 +2733,8 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
-      <c r="B40" s="60"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="62"/>
       <c r="C40" s="19" t="s">
         <v>32</v>
       </c>
@@ -2730,8 +2758,8 @@
         <f t="shared" si="6"/>
         <v>7.9743999999999995E-2</v>
       </c>
-      <c r="K40" s="59"/>
-      <c r="L40" s="60"/>
+      <c r="K40" s="61"/>
+      <c r="L40" s="62"/>
       <c r="M40" s="19" t="s">
         <v>32</v>
       </c>
@@ -2757,10 +2785,10 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="61">
+      <c r="A41" s="42">
         <v>1280</v>
       </c>
-      <c r="B41" s="62"/>
+      <c r="B41" s="43"/>
       <c r="C41" s="4" t="s">
         <v>23</v>
       </c>
@@ -2778,10 +2806,10 @@
       </c>
       <c r="H41" s="5"/>
       <c r="J41" s="24"/>
-      <c r="K41" s="61">
+      <c r="K41" s="42">
         <v>1280</v>
       </c>
-      <c r="L41" s="62"/>
+      <c r="L41" s="43"/>
       <c r="M41" s="4" t="s">
         <v>23</v>
       </c>
@@ -2802,8 +2830,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="63"/>
-      <c r="B42" s="64"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="45"/>
       <c r="C42" s="4" t="s">
         <v>24</v>
       </c>
@@ -2820,8 +2848,8 @@
         <v>9.476E-3</v>
       </c>
       <c r="H42" s="5"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="64"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="45"/>
       <c r="M42" s="4" t="s">
         <v>24</v>
       </c>
@@ -2842,8 +2870,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="63"/>
-      <c r="B43" s="64"/>
+      <c r="A43" s="44"/>
+      <c r="B43" s="45"/>
       <c r="C43" s="19" t="s">
         <v>32</v>
       </c>
@@ -2864,8 +2892,8 @@
         <v>2.7875999999999998E-2</v>
       </c>
       <c r="H43" s="5"/>
-      <c r="K43" s="63"/>
-      <c r="L43" s="64"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="45"/>
       <c r="M43" s="19" t="s">
         <v>32</v>
       </c>
@@ -2891,8 +2919,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="63"/>
-      <c r="B44" s="64"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="4" t="s">
         <v>25</v>
       </c>
@@ -2910,8 +2938,8 @@
       </c>
       <c r="H44" s="5"/>
       <c r="J44" s="24"/>
-      <c r="K44" s="63"/>
-      <c r="L44" s="64"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="45"/>
       <c r="M44" s="4" t="s">
         <v>25</v>
       </c>
@@ -2932,8 +2960,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="63"/>
-      <c r="B45" s="64"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="4" t="s">
         <v>26</v>
       </c>
@@ -2950,8 +2978,8 @@
         <v>4.3580000000000001E-2</v>
       </c>
       <c r="H45" s="5"/>
-      <c r="K45" s="63"/>
-      <c r="L45" s="64"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="45"/>
       <c r="M45" s="4" t="s">
         <v>26</v>
       </c>
@@ -2972,8 +3000,8 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="65"/>
-      <c r="B46" s="66"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="47"/>
       <c r="C46" s="19" t="s">
         <v>32</v>
       </c>
@@ -2994,8 +3022,8 @@
         <v>0.146428</v>
       </c>
       <c r="H46" s="5"/>
-      <c r="K46" s="65"/>
-      <c r="L46" s="66"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="47"/>
       <c r="M46" s="19" t="s">
         <v>32</v>
       </c>
@@ -3021,10 +3049,10 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="42">
+      <c r="A47" s="63">
         <v>1345</v>
       </c>
-      <c r="B47" s="43"/>
+      <c r="B47" s="64"/>
       <c r="C47" s="7" t="s">
         <v>23</v>
       </c>
@@ -3042,10 +3070,10 @@
       </c>
       <c r="H47" s="5"/>
       <c r="J47" s="24"/>
-      <c r="K47" s="42">
+      <c r="K47" s="63">
         <v>1345</v>
       </c>
-      <c r="L47" s="43"/>
+      <c r="L47" s="64"/>
       <c r="M47" s="7" t="s">
         <v>23</v>
       </c>
@@ -3066,8 +3094,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="65"/>
+      <c r="B48" s="66"/>
       <c r="C48" s="7" t="s">
         <v>24</v>
       </c>
@@ -3084,8 +3112,8 @@
         <v>9.9319999999999999E-3</v>
       </c>
       <c r="H48" s="5"/>
-      <c r="K48" s="44"/>
-      <c r="L48" s="45"/>
+      <c r="K48" s="65"/>
+      <c r="L48" s="66"/>
       <c r="M48" s="7" t="s">
         <v>24</v>
       </c>
@@ -3104,8 +3132,8 @@
       <c r="R48" s="5"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
-      <c r="B49" s="45"/>
+      <c r="A49" s="65"/>
+      <c r="B49" s="66"/>
       <c r="C49" s="19" t="s">
         <v>32</v>
       </c>
@@ -3126,8 +3154,8 @@
         <v>2.8931999999999999E-2</v>
       </c>
       <c r="H49" s="5"/>
-      <c r="K49" s="44"/>
-      <c r="L49" s="45"/>
+      <c r="K49" s="65"/>
+      <c r="L49" s="66"/>
       <c r="M49" s="19" t="s">
         <v>32</v>
       </c>
@@ -3150,8 +3178,8 @@
       <c r="R49" s="5"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="45"/>
+      <c r="A50" s="65"/>
+      <c r="B50" s="66"/>
       <c r="C50" s="7" t="s">
         <v>25</v>
       </c>
@@ -3169,8 +3197,8 @@
       </c>
       <c r="H50" s="5"/>
       <c r="J50" s="24"/>
-      <c r="K50" s="44"/>
-      <c r="L50" s="45"/>
+      <c r="K50" s="65"/>
+      <c r="L50" s="66"/>
       <c r="M50" s="7" t="s">
         <v>25</v>
       </c>
@@ -3189,8 +3217,8 @@
       <c r="R50" s="5"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
-      <c r="B51" s="45"/>
+      <c r="A51" s="65"/>
+      <c r="B51" s="66"/>
       <c r="C51" s="7" t="s">
         <v>26</v>
       </c>
@@ -3207,8 +3235,8 @@
         <v>4.5887999999999998E-2</v>
       </c>
       <c r="H51" s="5"/>
-      <c r="K51" s="44"/>
-      <c r="L51" s="45"/>
+      <c r="K51" s="65"/>
+      <c r="L51" s="66"/>
       <c r="M51" s="7" t="s">
         <v>26</v>
       </c>
@@ -3227,8 +3255,8 @@
       <c r="R51" s="5"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="46"/>
-      <c r="B52" s="47"/>
+      <c r="A52" s="67"/>
+      <c r="B52" s="68"/>
       <c r="C52" s="19" t="s">
         <v>32</v>
       </c>
@@ -3249,8 +3277,8 @@
         <v>0.15465999999999999</v>
       </c>
       <c r="H52" s="5"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="47"/>
+      <c r="K52" s="67"/>
+      <c r="L52" s="68"/>
       <c r="M52" s="19" t="s">
         <v>32</v>
       </c>
@@ -3274,13 +3302,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="K41:L46"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L8"/>
-    <mergeCell ref="K9:L13"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="K47:L52"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="A47:B52"/>
@@ -3297,6 +3318,13 @@
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="K29:L34"/>
     <mergeCell ref="K35:L40"/>
+    <mergeCell ref="K41:L46"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L8"/>
+    <mergeCell ref="K9:L13"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3304,11 +3332,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView topLeftCell="G37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3334,32 +3362,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="68"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15" t="s">
         <v>1</v>
@@ -3411,10 +3439,10 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="49">
+      <c r="A3" s="51">
         <v>584</v>
       </c>
-      <c r="B3" s="50"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
@@ -3468,8 +3496,8 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
@@ -3523,8 +3551,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -3594,8 +3622,8 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
@@ -3649,8 +3677,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="54"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
@@ -3720,10 +3748,10 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="55">
+      <c r="A8" s="57">
         <v>980</v>
       </c>
-      <c r="B8" s="56"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="16" t="s">
         <v>30</v>
       </c>
@@ -3774,8 +3802,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="58"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
@@ -3829,8 +3857,8 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="58"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="16" t="s">
         <v>35</v>
       </c>
@@ -3896,8 +3924,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="16" t="s">
         <v>22</v>
       </c>
@@ -3951,8 +3979,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="60"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="16" t="s">
         <v>34</v>
       </c>
@@ -4018,10 +4046,10 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="61">
+      <c r="A13" s="42">
         <v>1280</v>
       </c>
-      <c r="B13" s="62"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
@@ -4072,8 +4100,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="63"/>
-      <c r="B14" s="64"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
@@ -4127,8 +4155,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="64"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
@@ -4194,8 +4222,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="63"/>
-      <c r="B16" s="64"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
@@ -4249,8 +4277,8 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
-      <c r="B17" s="66"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
@@ -4316,10 +4344,10 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="42">
+      <c r="A18" s="63">
         <v>1345</v>
       </c>
-      <c r="B18" s="43"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="7" t="s">
         <v>30</v>
       </c>
@@ -4373,8 +4401,8 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="7" t="s">
         <v>21</v>
       </c>
@@ -4431,8 +4459,8 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="7" t="s">
         <v>35</v>
       </c>
@@ -4498,8 +4526,8 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="7" t="s">
         <v>22</v>
       </c>
@@ -4553,8 +4581,8 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
@@ -4859,10 +4887,10 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="68"/>
+      <c r="B33" s="50"/>
       <c r="C33" s="14"/>
       <c r="D33" s="15" t="s">
         <v>1</v>
@@ -4911,10 +4939,10 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="49">
+      <c r="A34" s="51">
         <v>584</v>
       </c>
-      <c r="B34" s="50"/>
+      <c r="B34" s="52"/>
       <c r="C34" s="1" t="s">
         <v>23</v>
       </c>
@@ -4965,8 +4993,8 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="51"/>
-      <c r="B35" s="52"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
@@ -5017,8 +5045,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
-      <c r="B36" s="52"/>
+      <c r="A36" s="53"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="19" t="s">
         <v>32</v>
       </c>
@@ -5084,8 +5112,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="51"/>
-      <c r="B37" s="52"/>
+      <c r="A37" s="53"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="1" t="s">
         <v>25</v>
       </c>
@@ -5136,8 +5164,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="51"/>
-      <c r="B38" s="52"/>
+      <c r="A38" s="53"/>
+      <c r="B38" s="54"/>
       <c r="C38" s="1" t="s">
         <v>26</v>
       </c>
@@ -5188,8 +5216,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="53"/>
-      <c r="B39" s="54"/>
+      <c r="A39" s="55"/>
+      <c r="B39" s="56"/>
       <c r="C39" s="19" t="s">
         <v>32</v>
       </c>
@@ -5255,10 +5283,10 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="55">
+      <c r="A40" s="57">
         <v>980</v>
       </c>
-      <c r="B40" s="56"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="16" t="s">
         <v>23</v>
       </c>
@@ -5309,8 +5337,8 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="57"/>
-      <c r="B41" s="58"/>
+      <c r="A41" s="59"/>
+      <c r="B41" s="60"/>
       <c r="C41" s="16" t="s">
         <v>24</v>
       </c>
@@ -5361,8 +5389,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="57"/>
-      <c r="B42" s="58"/>
+      <c r="A42" s="59"/>
+      <c r="B42" s="60"/>
       <c r="C42" s="19" t="s">
         <v>32</v>
       </c>
@@ -5428,8 +5456,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="57"/>
-      <c r="B43" s="58"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="60"/>
       <c r="C43" s="16" t="s">
         <v>25</v>
       </c>
@@ -5480,8 +5508,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="57"/>
-      <c r="B44" s="58"/>
+      <c r="A44" s="59"/>
+      <c r="B44" s="60"/>
       <c r="C44" s="16" t="s">
         <v>26</v>
       </c>
@@ -5532,8 +5560,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
-      <c r="B45" s="60"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="62"/>
       <c r="C45" s="19" t="s">
         <v>32</v>
       </c>
@@ -5599,10 +5627,10 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="61">
+      <c r="A46" s="42">
         <v>1280</v>
       </c>
-      <c r="B46" s="62"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="4" t="s">
         <v>23</v>
       </c>
@@ -5653,8 +5681,8 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="63"/>
-      <c r="B47" s="64"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="45"/>
       <c r="C47" s="4" t="s">
         <v>24</v>
       </c>
@@ -5705,8 +5733,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="63"/>
-      <c r="B48" s="64"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="19" t="s">
         <v>32</v>
       </c>
@@ -5772,8 +5800,8 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="63"/>
-      <c r="B49" s="64"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="4" t="s">
         <v>25</v>
       </c>
@@ -5824,8 +5852,8 @@
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="63"/>
-      <c r="B50" s="64"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="45"/>
       <c r="C50" s="4" t="s">
         <v>26</v>
       </c>
@@ -5876,8 +5904,8 @@
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="65"/>
-      <c r="B51" s="66"/>
+      <c r="A51" s="46"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="19" t="s">
         <v>32</v>
       </c>
@@ -5943,10 +5971,10 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="42">
+      <c r="A52" s="63">
         <v>1345</v>
       </c>
-      <c r="B52" s="43"/>
+      <c r="B52" s="64"/>
       <c r="C52" s="7" t="s">
         <v>23</v>
       </c>
@@ -5997,8 +6025,8 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
-      <c r="B53" s="45"/>
+      <c r="A53" s="65"/>
+      <c r="B53" s="66"/>
       <c r="C53" s="7" t="s">
         <v>24</v>
       </c>
@@ -6049,8 +6077,8 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="45"/>
+      <c r="A54" s="65"/>
+      <c r="B54" s="66"/>
       <c r="C54" s="19" t="s">
         <v>32</v>
       </c>
@@ -6116,8 +6144,8 @@
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="45"/>
+      <c r="A55" s="65"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="7" t="s">
         <v>25</v>
       </c>
@@ -6168,8 +6196,8 @@
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="45"/>
+      <c r="A56" s="65"/>
+      <c r="B56" s="66"/>
       <c r="C56" s="7" t="s">
         <v>26</v>
       </c>
@@ -6220,8 +6248,8 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="46"/>
-      <c r="B57" s="47"/>
+      <c r="A57" s="67"/>
+      <c r="B57" s="68"/>
       <c r="C57" s="19" t="s">
         <v>32</v>
       </c>
@@ -6306,7 +6334,239 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C7:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="91" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="91">
+        <v>1</v>
+      </c>
+      <c r="E7" s="91">
+        <v>2</v>
+      </c>
+      <c r="F7" s="91">
+        <v>3</v>
+      </c>
+      <c r="G7" s="91">
+        <v>4</v>
+      </c>
+      <c r="H7" s="91">
+        <v>5</v>
+      </c>
+      <c r="I7" s="91">
+        <v>6</v>
+      </c>
+      <c r="J7" s="91">
+        <v>7</v>
+      </c>
+      <c r="K7" s="91">
+        <v>8</v>
+      </c>
+      <c r="L7" s="91">
+        <v>9</v>
+      </c>
+      <c r="M7" s="91">
+        <v>10</v>
+      </c>
+      <c r="N7" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="O7" s="91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8">
+        <v>41</v>
+      </c>
+      <c r="E8">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <v>41</v>
+      </c>
+      <c r="G8">
+        <v>41</v>
+      </c>
+      <c r="H8">
+        <v>41</v>
+      </c>
+      <c r="I8">
+        <v>41</v>
+      </c>
+      <c r="J8">
+        <v>41</v>
+      </c>
+      <c r="K8">
+        <v>41</v>
+      </c>
+      <c r="L8">
+        <v>41</v>
+      </c>
+      <c r="M8">
+        <v>41</v>
+      </c>
+      <c r="N8">
+        <f>SUM(D8:M8)</f>
+        <v>410</v>
+      </c>
+      <c r="O8" s="92">
+        <f>N8/410</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <v>41</v>
+      </c>
+      <c r="G9">
+        <v>41</v>
+      </c>
+      <c r="H9">
+        <v>41</v>
+      </c>
+      <c r="I9">
+        <v>41</v>
+      </c>
+      <c r="J9">
+        <v>41</v>
+      </c>
+      <c r="K9">
+        <v>41</v>
+      </c>
+      <c r="L9">
+        <v>41</v>
+      </c>
+      <c r="M9">
+        <v>41</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9:N11" si="0">SUM(D9:M9)</f>
+        <v>410</v>
+      </c>
+      <c r="O9" s="92">
+        <f t="shared" ref="O9:O11" si="1">N9/410</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>39</v>
+      </c>
+      <c r="G10">
+        <v>38</v>
+      </c>
+      <c r="H10">
+        <v>36</v>
+      </c>
+      <c r="I10">
+        <v>35</v>
+      </c>
+      <c r="J10">
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <v>38</v>
+      </c>
+      <c r="L10">
+        <v>27</v>
+      </c>
+      <c r="M10">
+        <v>27</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>356</v>
+      </c>
+      <c r="O10" s="92">
+        <f t="shared" si="1"/>
+        <v>0.86829268292682926</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>32</v>
+      </c>
+      <c r="F11">
+        <v>37</v>
+      </c>
+      <c r="G11">
+        <v>38</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+      <c r="I11">
+        <v>34</v>
+      </c>
+      <c r="J11">
+        <v>26</v>
+      </c>
+      <c r="K11">
+        <v>20</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <v>29</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>285</v>
+      </c>
+      <c r="O11" s="92">
+        <f t="shared" si="1"/>
+        <v>0.69512195121951215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:R38"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -6380,7 +6640,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="79">
+      <c r="B8" s="86">
         <v>584</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -6401,7 +6661,7 @@
       <c r="H8" s="1">
         <v>8.0800000000000004E-3</v>
       </c>
-      <c r="L8" s="80">
+      <c r="L8" s="76">
         <v>584</v>
       </c>
       <c r="M8" s="1" t="s">
@@ -6424,7 +6684,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="79"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="1" t="s">
         <v>68</v>
       </c>
@@ -6443,7 +6703,7 @@
       <c r="H9" s="1">
         <v>4.5935999999999998E-2</v>
       </c>
-      <c r="L9" s="81"/>
+      <c r="L9" s="77"/>
       <c r="M9" s="1" t="s">
         <v>65</v>
       </c>
@@ -6469,7 +6729,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="76">
+      <c r="B10" s="87">
         <v>980</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -6490,7 +6750,7 @@
       <c r="H10" s="16">
         <v>1.2456E-2</v>
       </c>
-      <c r="L10" s="81"/>
+      <c r="L10" s="77"/>
       <c r="M10" s="1" t="s">
         <v>61</v>
       </c>
@@ -6511,7 +6771,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="76"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="16" t="s">
         <v>68</v>
       </c>
@@ -6530,7 +6790,7 @@
       <c r="H11" s="16">
         <v>6.3119999999999996E-2</v>
       </c>
-      <c r="L11" s="82"/>
+      <c r="L11" s="78"/>
       <c r="M11" s="1" t="s">
         <v>66</v>
       </c>
@@ -6556,7 +6816,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="77">
+      <c r="B12" s="88">
         <v>1280</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -6577,7 +6837,7 @@
       <c r="H12" s="4">
         <v>1.5299999999999999E-2</v>
       </c>
-      <c r="L12" s="83">
+      <c r="L12" s="79">
         <v>980</v>
       </c>
       <c r="M12" s="16" t="s">
@@ -6600,7 +6860,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="77"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="4" t="s">
         <v>68</v>
       </c>
@@ -6619,7 +6879,7 @@
       <c r="H13" s="4">
         <v>6.6844000000000001E-2</v>
       </c>
-      <c r="L13" s="84"/>
+      <c r="L13" s="80"/>
       <c r="M13" s="16" t="s">
         <v>66</v>
       </c>
@@ -6645,7 +6905,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="78">
+      <c r="B14" s="85">
         <v>1345</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -6666,7 +6926,7 @@
       <c r="H14" s="7">
         <v>1.5807999999999999E-2</v>
       </c>
-      <c r="L14" s="84"/>
+      <c r="L14" s="80"/>
       <c r="M14" s="16" t="s">
         <v>61</v>
       </c>
@@ -6687,7 +6947,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="78"/>
+      <c r="B15" s="85"/>
       <c r="C15" s="7" t="s">
         <v>68</v>
       </c>
@@ -6706,7 +6966,7 @@
       <c r="H15" s="7">
         <v>6.7227999999999996E-2</v>
       </c>
-      <c r="L15" s="85"/>
+      <c r="L15" s="81"/>
       <c r="M15" s="16" t="s">
         <v>66</v>
       </c>
@@ -6732,7 +6992,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L16" s="86">
+      <c r="L16" s="82">
         <v>1280</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -6755,7 +7015,7 @@
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L17" s="87"/>
+      <c r="L17" s="83"/>
       <c r="M17" s="4" t="s">
         <v>65</v>
       </c>
@@ -6781,7 +7041,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L18" s="87"/>
+      <c r="L18" s="83"/>
       <c r="M18" s="4" t="s">
         <v>61</v>
       </c>
@@ -6802,7 +7062,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L19" s="88"/>
+      <c r="L19" s="84"/>
       <c r="M19" s="4" t="s">
         <v>65</v>
       </c>
@@ -6828,7 +7088,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L20" s="78">
+      <c r="L20" s="85">
         <v>1345</v>
       </c>
       <c r="M20" s="7" t="s">
@@ -6851,7 +7111,7 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L21" s="78"/>
+      <c r="L21" s="85"/>
       <c r="M21" s="7" t="s">
         <v>65</v>
       </c>
@@ -6877,7 +7137,7 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L22" s="78"/>
+      <c r="L22" s="85"/>
       <c r="M22" s="7" t="s">
         <v>61</v>
       </c>
@@ -6898,7 +7158,7 @@
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L23" s="78"/>
+      <c r="L23" s="85"/>
       <c r="M23" s="7" t="s">
         <v>65</v>
       </c>
@@ -6952,7 +7212,7 @@
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="79">
+      <c r="B31" s="86">
         <v>584</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -6975,7 +7235,7 @@
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="79"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="1" t="s">
         <v>68</v>
       </c>
@@ -6996,7 +7256,7 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="76">
+      <c r="B33" s="87">
         <v>980</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -7019,7 +7279,7 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="76"/>
+      <c r="B34" s="87"/>
       <c r="C34" s="16" t="s">
         <v>68</v>
       </c>
@@ -7040,7 +7300,7 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="77">
+      <c r="B35" s="88">
         <v>1280</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -7063,7 +7323,7 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="77"/>
+      <c r="B36" s="88"/>
       <c r="C36" s="4" t="s">
         <v>68</v>
       </c>
@@ -7084,7 +7344,7 @@
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="78">
+      <c r="B37" s="85">
         <v>1345</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -7107,7 +7367,7 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="78"/>
+      <c r="B38" s="85"/>
       <c r="C38" s="7" t="s">
         <v>68</v>
       </c>
@@ -7129,11 +7389,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="B31:B32"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
@@ -7141,14 +7396,19 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B15"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679D130C-42BE-4E6B-A6EF-80A1FFE77484}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:R19"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">

</xml_diff>